<commit_message>
changes for revised version
</commit_message>
<xml_diff>
--- a/data/supplementary_data/SupplementaryTable5.xlsx
+++ b/data/supplementary_data/SupplementaryTable5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\postdoc\papers\insulators\data\supplementary_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\papers\insulators\data\supplementary_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3923079A-4CAA-4E11-839A-6828E81465CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4959E62D-487C-44C8-9095-DDC6E5ACFD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insulator fragments" sheetId="1" r:id="rId1"/>
@@ -951,7 +951,18 @@
     <t>CATCGGGGAAGGCTGGGGACAGGGAGGCCGAGG</t>
   </si>
   <si>
-    <t>Supplementary Table 5 | Oligonucleotides used in this study.</t>
+    <r>
+      <t>Supplementary Table 5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Oligonucleotides used in this study.</t>
+    </r>
   </si>
 </sst>
 </file>

</xml_diff>